<commit_message>
refactor: Prioritize loading combined data, updated target university, and improve README formatting.
</commit_message>
<xml_diff>
--- a/Data_PTN_BLU_Gabungan_Final.xlsx
+++ b/Data_PTN_BLU_Gabungan_Final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1980"/>
+  <dimension ref="A1:L2029"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -99445,6 +99445,2456 @@
         </is>
       </c>
     </row>
+    <row r="1981">
+      <c r="A1981" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1981" t="n">
+        <v>86104</v>
+      </c>
+      <c r="C1981" t="inlineStr">
+        <is>
+          <t>Administrasi Pendidikan</t>
+        </is>
+      </c>
+      <c r="D1981" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1981" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F1981" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G1981" t="n">
+        <v>7</v>
+      </c>
+      <c r="H1981" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1981" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1981" t="n">
+        <v>7</v>
+      </c>
+      <c r="K1981" t="n">
+        <v>45</v>
+      </c>
+      <c r="L1981" t="inlineStr">
+        <is>
+          <t>1:6.43</t>
+        </is>
+      </c>
+    </row>
+    <row r="1982">
+      <c r="A1982" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1982" t="n">
+        <v>13261</v>
+      </c>
+      <c r="C1982" t="inlineStr">
+        <is>
+          <t>Administrasi Rumah Sakit</t>
+        </is>
+      </c>
+      <c r="D1982" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1982" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1982" t="inlineStr">
+        <is>
+          <t>Terakreditasi</t>
+        </is>
+      </c>
+      <c r="G1982" t="n">
+        <v>14</v>
+      </c>
+      <c r="H1982" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1982" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1982" t="n">
+        <v>7</v>
+      </c>
+      <c r="K1982" t="n">
+        <v>128</v>
+      </c>
+      <c r="L1982" t="inlineStr">
+        <is>
+          <t>1:9.14</t>
+        </is>
+      </c>
+    </row>
+    <row r="1983">
+      <c r="A1983" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1983" t="n">
+        <v>54201</v>
+      </c>
+      <c r="C1983" t="inlineStr">
+        <is>
+          <t>Agribisnis</t>
+        </is>
+      </c>
+      <c r="D1983" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1983" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1983" t="inlineStr">
+        <is>
+          <t>Unggul</t>
+        </is>
+      </c>
+      <c r="G1983" t="n">
+        <v>41</v>
+      </c>
+      <c r="H1983" t="n">
+        <v>18</v>
+      </c>
+      <c r="I1983" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1983" t="n">
+        <v>18</v>
+      </c>
+      <c r="K1983" t="n">
+        <v>585</v>
+      </c>
+      <c r="L1983" t="inlineStr">
+        <is>
+          <t>1:14.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="1984">
+      <c r="A1984" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1984" t="n">
+        <v>54211</v>
+      </c>
+      <c r="C1984" t="inlineStr">
+        <is>
+          <t>Agroteknologi</t>
+        </is>
+      </c>
+      <c r="D1984" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1984" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1984" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G1984" t="n">
+        <v>54</v>
+      </c>
+      <c r="H1984" t="n">
+        <v>27</v>
+      </c>
+      <c r="I1984" t="n">
+        <v>4</v>
+      </c>
+      <c r="J1984" t="n">
+        <v>31</v>
+      </c>
+      <c r="K1984" t="n">
+        <v>721</v>
+      </c>
+      <c r="L1984" t="inlineStr">
+        <is>
+          <t>1:13.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1985">
+      <c r="A1985" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1985" t="n">
+        <v>62401</v>
+      </c>
+      <c r="C1985" t="inlineStr">
+        <is>
+          <t>Akuntansi</t>
+        </is>
+      </c>
+      <c r="D1985" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1985" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+      <c r="F1985" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G1985" t="n">
+        <v>21</v>
+      </c>
+      <c r="H1985" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1985" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1985" t="n">
+        <v>7</v>
+      </c>
+      <c r="K1985" t="n">
+        <v>197</v>
+      </c>
+      <c r="L1985" t="inlineStr">
+        <is>
+          <t>1:9.38</t>
+        </is>
+      </c>
+    </row>
+    <row r="1986">
+      <c r="A1986" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1986" t="n">
+        <v>62201</v>
+      </c>
+      <c r="C1986" t="inlineStr">
+        <is>
+          <t>Akuntansi</t>
+        </is>
+      </c>
+      <c r="D1986" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1986" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1986" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G1986" t="n">
+        <v>58</v>
+      </c>
+      <c r="H1986" t="n">
+        <v>27</v>
+      </c>
+      <c r="I1986" t="n">
+        <v>4</v>
+      </c>
+      <c r="J1986" t="n">
+        <v>31</v>
+      </c>
+      <c r="K1986" t="n">
+        <v>1054</v>
+      </c>
+      <c r="L1986" t="inlineStr">
+        <is>
+          <t>1:18.17</t>
+        </is>
+      </c>
+    </row>
+    <row r="1987">
+      <c r="A1987" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1987" t="n">
+        <v>23201</v>
+      </c>
+      <c r="C1987" t="inlineStr">
+        <is>
+          <t>Arsitektur</t>
+        </is>
+      </c>
+      <c r="D1987" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1987" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1987" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1987" t="n">
+        <v>0</v>
+      </c>
+      <c r="H1987" t="n">
+        <v>5</v>
+      </c>
+      <c r="I1987" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1987" t="n">
+        <v>5</v>
+      </c>
+      <c r="K1987" t="n">
+        <v>0</v>
+      </c>
+      <c r="L1987" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="1988">
+      <c r="A1988" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1988" t="n">
+        <v>48201</v>
+      </c>
+      <c r="C1988" t="inlineStr">
+        <is>
+          <t>Farmasi</t>
+        </is>
+      </c>
+      <c r="D1988" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1988" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1988" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G1988" t="n">
+        <v>23</v>
+      </c>
+      <c r="H1988" t="n">
+        <v>14</v>
+      </c>
+      <c r="I1988" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1988" t="n">
+        <v>14</v>
+      </c>
+      <c r="K1988" t="n">
+        <v>310</v>
+      </c>
+      <c r="L1988" t="inlineStr">
+        <is>
+          <t>1:13.48</t>
+        </is>
+      </c>
+    </row>
+    <row r="1989">
+      <c r="A1989" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1989" t="n">
+        <v>45201</v>
+      </c>
+      <c r="C1989" t="inlineStr">
+        <is>
+          <t>Fisika</t>
+        </is>
+      </c>
+      <c r="D1989" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1989" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1989" t="inlineStr">
+        <is>
+          <t>Baik</t>
+        </is>
+      </c>
+      <c r="G1989" t="n">
+        <v>10</v>
+      </c>
+      <c r="H1989" t="n">
+        <v>8</v>
+      </c>
+      <c r="I1989" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1989" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1989" t="n">
+        <v>57</v>
+      </c>
+      <c r="L1989" t="inlineStr">
+        <is>
+          <t>1:5.7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1990">
+      <c r="A1990" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1990" t="n">
+        <v>13211</v>
+      </c>
+      <c r="C1990" t="inlineStr">
+        <is>
+          <t>Gizi</t>
+        </is>
+      </c>
+      <c r="D1990" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1990" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1990" t="inlineStr">
+        <is>
+          <t>Baik</t>
+        </is>
+      </c>
+      <c r="G1990" t="n">
+        <v>21</v>
+      </c>
+      <c r="H1990" t="n">
+        <v>14</v>
+      </c>
+      <c r="I1990" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1990" t="n">
+        <v>14</v>
+      </c>
+      <c r="K1990" t="n">
+        <v>298</v>
+      </c>
+      <c r="L1990" t="inlineStr">
+        <is>
+          <t>1:14.19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1991">
+      <c r="A1991" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1991" t="n">
+        <v>64201</v>
+      </c>
+      <c r="C1991" t="inlineStr">
+        <is>
+          <t>Hubungan Internasional</t>
+        </is>
+      </c>
+      <c r="D1991" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1991" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1991" t="inlineStr">
+        <is>
+          <t>Baik</t>
+        </is>
+      </c>
+      <c r="G1991" t="n">
+        <v>16</v>
+      </c>
+      <c r="H1991" t="n">
+        <v>10</v>
+      </c>
+      <c r="I1991" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1991" t="n">
+        <v>10</v>
+      </c>
+      <c r="K1991" t="n">
+        <v>289</v>
+      </c>
+      <c r="L1991" t="inlineStr">
+        <is>
+          <t>1:18.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1992">
+      <c r="A1992" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1992" t="n">
+        <v>74101</v>
+      </c>
+      <c r="C1992" t="inlineStr">
+        <is>
+          <t>Ilmu Hukum</t>
+        </is>
+      </c>
+      <c r="D1992" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1992" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F1992" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G1992" t="n">
+        <v>12</v>
+      </c>
+      <c r="H1992" t="n">
+        <v>8</v>
+      </c>
+      <c r="I1992" t="n">
+        <v>2</v>
+      </c>
+      <c r="J1992" t="n">
+        <v>10</v>
+      </c>
+      <c r="K1992" t="n">
+        <v>78</v>
+      </c>
+      <c r="L1992" t="inlineStr">
+        <is>
+          <t>1:6.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1993">
+      <c r="A1993" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1993" t="n">
+        <v>74201</v>
+      </c>
+      <c r="C1993" t="inlineStr">
+        <is>
+          <t>Ilmu Hukum</t>
+        </is>
+      </c>
+      <c r="D1993" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1993" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1993" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G1993" t="n">
+        <v>56</v>
+      </c>
+      <c r="H1993" t="n">
+        <v>36</v>
+      </c>
+      <c r="I1993" t="n">
+        <v>6</v>
+      </c>
+      <c r="J1993" t="n">
+        <v>42</v>
+      </c>
+      <c r="K1993" t="n">
+        <v>1176</v>
+      </c>
+      <c r="L1993" t="inlineStr">
+        <is>
+          <t>1:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1994">
+      <c r="A1994" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1994" t="n">
+        <v>89201</v>
+      </c>
+      <c r="C1994" t="inlineStr">
+        <is>
+          <t>Ilmu Keolahragaan</t>
+        </is>
+      </c>
+      <c r="D1994" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1994" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1994" t="inlineStr">
+        <is>
+          <t>Baik</t>
+        </is>
+      </c>
+      <c r="G1994" t="n">
+        <v>25</v>
+      </c>
+      <c r="H1994" t="n">
+        <v>12</v>
+      </c>
+      <c r="I1994" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1994" t="n">
+        <v>12</v>
+      </c>
+      <c r="K1994" t="n">
+        <v>289</v>
+      </c>
+      <c r="L1994" t="inlineStr">
+        <is>
+          <t>1:11.56</t>
+        </is>
+      </c>
+    </row>
+    <row r="1995">
+      <c r="A1995" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1995" t="n">
+        <v>70101</v>
+      </c>
+      <c r="C1995" t="inlineStr">
+        <is>
+          <t>Ilmu Komunikasi</t>
+        </is>
+      </c>
+      <c r="D1995" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1995" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F1995" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G1995" t="n">
+        <v>9</v>
+      </c>
+      <c r="H1995" t="n">
+        <v>5</v>
+      </c>
+      <c r="I1995" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1995" t="n">
+        <v>5</v>
+      </c>
+      <c r="K1995" t="n">
+        <v>15</v>
+      </c>
+      <c r="L1995" t="inlineStr">
+        <is>
+          <t>1:1.67</t>
+        </is>
+      </c>
+    </row>
+    <row r="1996">
+      <c r="A1996" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1996" t="n">
+        <v>70201</v>
+      </c>
+      <c r="C1996" t="inlineStr">
+        <is>
+          <t>Ilmu Komunikasi</t>
+        </is>
+      </c>
+      <c r="D1996" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1996" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1996" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G1996" t="n">
+        <v>31</v>
+      </c>
+      <c r="H1996" t="n">
+        <v>18</v>
+      </c>
+      <c r="I1996" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1996" t="n">
+        <v>19</v>
+      </c>
+      <c r="K1996" t="n">
+        <v>855</v>
+      </c>
+      <c r="L1996" t="inlineStr">
+        <is>
+          <t>1:27.58</t>
+        </is>
+      </c>
+    </row>
+    <row r="1997">
+      <c r="A1997" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1997" t="n">
+        <v>65201</v>
+      </c>
+      <c r="C1997" t="inlineStr">
+        <is>
+          <t>Ilmu Pemerintahan</t>
+        </is>
+      </c>
+      <c r="D1997" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1997" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1997" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G1997" t="n">
+        <v>31</v>
+      </c>
+      <c r="H1997" t="n">
+        <v>24</v>
+      </c>
+      <c r="I1997" t="n">
+        <v>2</v>
+      </c>
+      <c r="J1997" t="n">
+        <v>26</v>
+      </c>
+      <c r="K1997" t="n">
+        <v>824</v>
+      </c>
+      <c r="L1997" t="inlineStr">
+        <is>
+          <t>1:26.58</t>
+        </is>
+      </c>
+    </row>
+    <row r="1998">
+      <c r="A1998" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1998" t="n">
+        <v>54108</v>
+      </c>
+      <c r="C1998" t="inlineStr">
+        <is>
+          <t>Ilmu Pertanian</t>
+        </is>
+      </c>
+      <c r="D1998" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1998" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F1998" t="inlineStr">
+        <is>
+          <t>Terakreditasi Sementara</t>
+        </is>
+      </c>
+      <c r="G1998" t="n">
+        <v>12</v>
+      </c>
+      <c r="H1998" t="n">
+        <v>5</v>
+      </c>
+      <c r="I1998" t="n">
+        <v>1</v>
+      </c>
+      <c r="J1998" t="n">
+        <v>6</v>
+      </c>
+      <c r="K1998" t="n">
+        <v>13</v>
+      </c>
+      <c r="L1998" t="inlineStr">
+        <is>
+          <t>1:1.08</t>
+        </is>
+      </c>
+    </row>
+    <row r="1999">
+      <c r="A1999" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B1999" t="n">
+        <v>55202</v>
+      </c>
+      <c r="C1999" t="inlineStr">
+        <is>
+          <t>Informatika</t>
+        </is>
+      </c>
+      <c r="D1999" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E1999" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F1999" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G1999" t="n">
+        <v>33</v>
+      </c>
+      <c r="H1999" t="n">
+        <v>29</v>
+      </c>
+      <c r="I1999" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1999" t="n">
+        <v>29</v>
+      </c>
+      <c r="K1999" t="n">
+        <v>717</v>
+      </c>
+      <c r="L1999" t="inlineStr">
+        <is>
+          <t>1:21.73</t>
+        </is>
+      </c>
+    </row>
+    <row r="2000">
+      <c r="A2000" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2000" t="n">
+        <v>15401</v>
+      </c>
+      <c r="C2000" t="inlineStr">
+        <is>
+          <t>Kebidanan</t>
+        </is>
+      </c>
+      <c r="D2000" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2000" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+      <c r="F2000" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G2000" t="n">
+        <v>26</v>
+      </c>
+      <c r="H2000" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2000" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2000" t="n">
+        <v>9</v>
+      </c>
+      <c r="K2000" t="n">
+        <v>223</v>
+      </c>
+      <c r="L2000" t="inlineStr">
+        <is>
+          <t>1:8.58</t>
+        </is>
+      </c>
+    </row>
+    <row r="2001">
+      <c r="A2001" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2001" t="n">
+        <v>15201</v>
+      </c>
+      <c r="C2001" t="inlineStr">
+        <is>
+          <t>Kebidanan</t>
+        </is>
+      </c>
+      <c r="D2001" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2001" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2001" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2001" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2001" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2001" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2001" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2001" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2001" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="2002">
+      <c r="A2002" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2002" t="n">
+        <v>47201</v>
+      </c>
+      <c r="C2002" t="inlineStr">
+        <is>
+          <t>Kimia</t>
+        </is>
+      </c>
+      <c r="D2002" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2002" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2002" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2002" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2002" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2002" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2002" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2002" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2002" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="2003">
+      <c r="A2003" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2003" t="n">
+        <v>61101</v>
+      </c>
+      <c r="C2003" t="inlineStr">
+        <is>
+          <t>Manajemen</t>
+        </is>
+      </c>
+      <c r="D2003" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2003" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F2003" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G2003" t="n">
+        <v>8</v>
+      </c>
+      <c r="H2003" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2003" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2003" t="n">
+        <v>9</v>
+      </c>
+      <c r="K2003" t="n">
+        <v>61</v>
+      </c>
+      <c r="L2003" t="inlineStr">
+        <is>
+          <t>1:7.63</t>
+        </is>
+      </c>
+    </row>
+    <row r="2004">
+      <c r="A2004" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2004" t="n">
+        <v>61201</v>
+      </c>
+      <c r="C2004" t="inlineStr">
+        <is>
+          <t>Manajemen</t>
+        </is>
+      </c>
+      <c r="D2004" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2004" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2004" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G2004" t="n">
+        <v>62</v>
+      </c>
+      <c r="H2004" t="n">
+        <v>35</v>
+      </c>
+      <c r="I2004" t="n">
+        <v>2</v>
+      </c>
+      <c r="J2004" t="n">
+        <v>37</v>
+      </c>
+      <c r="K2004" t="n">
+        <v>1149</v>
+      </c>
+      <c r="L2004" t="inlineStr">
+        <is>
+          <t>1:18.53</t>
+        </is>
+      </c>
+    </row>
+    <row r="2005">
+      <c r="A2005" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2005" t="n">
+        <v>86231</v>
+      </c>
+      <c r="C2005" t="inlineStr">
+        <is>
+          <t>Manajemen Pendidikan Islam</t>
+        </is>
+      </c>
+      <c r="D2005" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2005" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2005" t="inlineStr">
+        <is>
+          <t>Unggul</t>
+        </is>
+      </c>
+      <c r="G2005" t="n">
+        <v>34</v>
+      </c>
+      <c r="H2005" t="n">
+        <v>15</v>
+      </c>
+      <c r="I2005" t="n">
+        <v>2</v>
+      </c>
+      <c r="J2005" t="n">
+        <v>17</v>
+      </c>
+      <c r="K2005" t="n">
+        <v>789</v>
+      </c>
+      <c r="L2005" t="inlineStr">
+        <is>
+          <t>1:23.21</t>
+        </is>
+      </c>
+    </row>
+    <row r="2006">
+      <c r="A2006" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2006" t="n">
+        <v>86130</v>
+      </c>
+      <c r="C2006" t="inlineStr">
+        <is>
+          <t>Pendidikan Agama Islam</t>
+        </is>
+      </c>
+      <c r="D2006" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2006" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F2006" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G2006" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2006" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2006" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2006" t="n">
+        <v>9</v>
+      </c>
+      <c r="K2006" t="n">
+        <v>35</v>
+      </c>
+      <c r="L2006" t="inlineStr">
+        <is>
+          <t>1:3.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="2007">
+      <c r="A2007" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2007" t="n">
+        <v>86208</v>
+      </c>
+      <c r="C2007" t="inlineStr">
+        <is>
+          <t>Pendidikan Agama Islam</t>
+        </is>
+      </c>
+      <c r="D2007" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2007" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2007" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G2007" t="n">
+        <v>40</v>
+      </c>
+      <c r="H2007" t="n">
+        <v>23</v>
+      </c>
+      <c r="I2007" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2007" t="n">
+        <v>24</v>
+      </c>
+      <c r="K2007" t="n">
+        <v>1155</v>
+      </c>
+      <c r="L2007" t="inlineStr">
+        <is>
+          <t>1:28.88</t>
+        </is>
+      </c>
+    </row>
+    <row r="2008">
+      <c r="A2008" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2008" t="n">
+        <v>88201</v>
+      </c>
+      <c r="C2008" t="inlineStr">
+        <is>
+          <t>Pendidikan Bahasa Dan Sastra Indonesia</t>
+        </is>
+      </c>
+      <c r="D2008" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2008" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2008" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G2008" t="n">
+        <v>34</v>
+      </c>
+      <c r="H2008" t="n">
+        <v>28</v>
+      </c>
+      <c r="I2008" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2008" t="n">
+        <v>28</v>
+      </c>
+      <c r="K2008" t="n">
+        <v>769</v>
+      </c>
+      <c r="L2008" t="inlineStr">
+        <is>
+          <t>1:22.62</t>
+        </is>
+      </c>
+    </row>
+    <row r="2009">
+      <c r="A2009" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2009" t="n">
+        <v>88203</v>
+      </c>
+      <c r="C2009" t="inlineStr">
+        <is>
+          <t>Pendidikan Bahasa Inggris</t>
+        </is>
+      </c>
+      <c r="D2009" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2009" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2009" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G2009" t="n">
+        <v>41</v>
+      </c>
+      <c r="H2009" t="n">
+        <v>32</v>
+      </c>
+      <c r="I2009" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2009" t="n">
+        <v>32</v>
+      </c>
+      <c r="K2009" t="n">
+        <v>790</v>
+      </c>
+      <c r="L2009" t="inlineStr">
+        <is>
+          <t>1:19.27</t>
+        </is>
+      </c>
+    </row>
+    <row r="2010">
+      <c r="A2010" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2010" t="n">
+        <v>86233</v>
+      </c>
+      <c r="C2010" t="inlineStr">
+        <is>
+          <t>Pendidikan Islam Anak Usia Dini</t>
+        </is>
+      </c>
+      <c r="D2010" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2010" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2010" t="inlineStr">
+        <is>
+          <t>Unggul</t>
+        </is>
+      </c>
+      <c r="G2010" t="n">
+        <v>19</v>
+      </c>
+      <c r="H2010" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2010" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2010" t="n">
+        <v>9</v>
+      </c>
+      <c r="K2010" t="n">
+        <v>223</v>
+      </c>
+      <c r="L2010" t="inlineStr">
+        <is>
+          <t>1:11.74</t>
+        </is>
+      </c>
+    </row>
+    <row r="2011">
+      <c r="A2011" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2011" t="n">
+        <v>85101</v>
+      </c>
+      <c r="C2011" t="inlineStr">
+        <is>
+          <t>Pendidikan Jasmani</t>
+        </is>
+      </c>
+      <c r="D2011" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2011" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F2011" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G2011" t="n">
+        <v>23</v>
+      </c>
+      <c r="H2011" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2011" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2011" t="n">
+        <v>6</v>
+      </c>
+      <c r="K2011" t="n">
+        <v>45</v>
+      </c>
+      <c r="L2011" t="inlineStr">
+        <is>
+          <t>1:1.96</t>
+        </is>
+      </c>
+    </row>
+    <row r="2012">
+      <c r="A2012" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2012" t="n">
+        <v>85201</v>
+      </c>
+      <c r="C2012" t="inlineStr">
+        <is>
+          <t>Pendidikan Jasmani Kesehatan &amp; Rekreasi</t>
+        </is>
+      </c>
+      <c r="D2012" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2012" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2012" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G2012" t="n">
+        <v>43</v>
+      </c>
+      <c r="H2012" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2012" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2012" t="n">
+        <v>27</v>
+      </c>
+      <c r="K2012" t="n">
+        <v>816</v>
+      </c>
+      <c r="L2012" t="inlineStr">
+        <is>
+          <t>1:18.98</t>
+        </is>
+      </c>
+    </row>
+    <row r="2013">
+      <c r="A2013" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2013" t="n">
+        <v>86205</v>
+      </c>
+      <c r="C2013" t="inlineStr">
+        <is>
+          <t>Pendidikan Luar Sekolah</t>
+        </is>
+      </c>
+      <c r="D2013" t="inlineStr">
+        <is>
+          <t>Alih Bentuk</t>
+        </is>
+      </c>
+      <c r="E2013" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2013" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2013" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2013" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2013" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2013" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2013" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2013" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="2014">
+      <c r="A2014" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2014" t="n">
+        <v>86205</v>
+      </c>
+      <c r="C2014" t="inlineStr">
+        <is>
+          <t>Pendidikan Masyarakat</t>
+        </is>
+      </c>
+      <c r="D2014" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2014" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2014" t="inlineStr">
+        <is>
+          <t>Unggul</t>
+        </is>
+      </c>
+      <c r="G2014" t="n">
+        <v>21</v>
+      </c>
+      <c r="H2014" t="n">
+        <v>16</v>
+      </c>
+      <c r="I2014" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2014" t="n">
+        <v>16</v>
+      </c>
+      <c r="K2014" t="n">
+        <v>391</v>
+      </c>
+      <c r="L2014" t="inlineStr">
+        <is>
+          <t>1:18.62</t>
+        </is>
+      </c>
+    </row>
+    <row r="2015">
+      <c r="A2015" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2015" t="n">
+        <v>84202</v>
+      </c>
+      <c r="C2015" t="inlineStr">
+        <is>
+          <t>Pendidikan Matematika</t>
+        </is>
+      </c>
+      <c r="D2015" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2015" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2015" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G2015" t="n">
+        <v>48</v>
+      </c>
+      <c r="H2015" t="n">
+        <v>32</v>
+      </c>
+      <c r="I2015" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2015" t="n">
+        <v>32</v>
+      </c>
+      <c r="K2015" t="n">
+        <v>664</v>
+      </c>
+      <c r="L2015" t="inlineStr">
+        <is>
+          <t>1:13.83</t>
+        </is>
+      </c>
+    </row>
+    <row r="2016">
+      <c r="A2016" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2016" t="n">
+        <v>84102</v>
+      </c>
+      <c r="C2016" t="inlineStr">
+        <is>
+          <t>Pendidikan Matematika</t>
+        </is>
+      </c>
+      <c r="D2016" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2016" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F2016" t="inlineStr">
+        <is>
+          <t>Baik</t>
+        </is>
+      </c>
+      <c r="G2016" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2016" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2016" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2016" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2016" t="n">
+        <v>36</v>
+      </c>
+      <c r="L2016" t="inlineStr">
+        <is>
+          <t>1:6</t>
+        </is>
+      </c>
+    </row>
+    <row r="2017">
+      <c r="A2017" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2017" t="n">
+        <v>15903</v>
+      </c>
+      <c r="C2017" t="inlineStr">
+        <is>
+          <t>Pendidikan Profesi Bidan</t>
+        </is>
+      </c>
+      <c r="D2017" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2017" t="inlineStr">
+        <is>
+          <t>Profesi</t>
+        </is>
+      </c>
+      <c r="F2017" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2017" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2017" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2017" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2017" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2017" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2017" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="2018">
+      <c r="A2018" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2018" t="n">
+        <v>86906</v>
+      </c>
+      <c r="C2018" t="inlineStr">
+        <is>
+          <t>Pendidikan Profesi Guru</t>
+        </is>
+      </c>
+      <c r="D2018" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2018" t="inlineStr">
+        <is>
+          <t>Profesi</t>
+        </is>
+      </c>
+      <c r="F2018" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G2018" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2018" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2018" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2018" t="n">
+        <v>7</v>
+      </c>
+      <c r="K2018" t="n">
+        <v>2575</v>
+      </c>
+      <c r="L2018" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="2019">
+      <c r="A2019" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2019" t="n">
+        <v>57201</v>
+      </c>
+      <c r="C2019" t="inlineStr">
+        <is>
+          <t>Sistem Informasi</t>
+        </is>
+      </c>
+      <c r="D2019" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2019" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2019" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G2019" t="n">
+        <v>35</v>
+      </c>
+      <c r="H2019" t="n">
+        <v>12</v>
+      </c>
+      <c r="I2019" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2019" t="n">
+        <v>12</v>
+      </c>
+      <c r="K2019" t="n">
+        <v>467</v>
+      </c>
+      <c r="L2019" t="inlineStr">
+        <is>
+          <t>1:13.34</t>
+        </is>
+      </c>
+    </row>
+    <row r="2020">
+      <c r="A2020" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2020" t="n">
+        <v>49201</v>
+      </c>
+      <c r="C2020" t="inlineStr">
+        <is>
+          <t>Statistika</t>
+        </is>
+      </c>
+      <c r="D2020" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2020" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2020" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2020" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2020" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2020" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2020" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2020" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2020" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="2021">
+      <c r="A2021" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2021" t="n">
+        <v>20201</v>
+      </c>
+      <c r="C2021" t="inlineStr">
+        <is>
+          <t>Teknik Elektro</t>
+        </is>
+      </c>
+      <c r="D2021" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2021" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2021" t="inlineStr">
+        <is>
+          <t>Terakreditasi Unggul</t>
+        </is>
+      </c>
+      <c r="G2021" t="n">
+        <v>27</v>
+      </c>
+      <c r="H2021" t="n">
+        <v>16</v>
+      </c>
+      <c r="I2021" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2021" t="n">
+        <v>16</v>
+      </c>
+      <c r="K2021" t="n">
+        <v>576</v>
+      </c>
+      <c r="L2021" t="inlineStr">
+        <is>
+          <t>1:21.33</t>
+        </is>
+      </c>
+    </row>
+    <row r="2022">
+      <c r="A2022" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2022" t="n">
+        <v>26201</v>
+      </c>
+      <c r="C2022" t="inlineStr">
+        <is>
+          <t>Teknik Industri</t>
+        </is>
+      </c>
+      <c r="D2022" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2022" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2022" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="G2022" t="n">
+        <v>34</v>
+      </c>
+      <c r="H2022" t="n">
+        <v>24</v>
+      </c>
+      <c r="I2022" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2022" t="n">
+        <v>24</v>
+      </c>
+      <c r="K2022" t="n">
+        <v>758</v>
+      </c>
+      <c r="L2022" t="inlineStr">
+        <is>
+          <t>1:22.29</t>
+        </is>
+      </c>
+    </row>
+    <row r="2023">
+      <c r="A2023" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2023" t="n">
+        <v>55201</v>
+      </c>
+      <c r="C2023" t="inlineStr">
+        <is>
+          <t>Teknik Informatika</t>
+        </is>
+      </c>
+      <c r="D2023" t="inlineStr">
+        <is>
+          <t>Alih Bentuk</t>
+        </is>
+      </c>
+      <c r="E2023" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2023" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2023" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2023" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2023" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2023" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2023" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2023" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="2024">
+      <c r="A2024" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2024" t="n">
+        <v>24201</v>
+      </c>
+      <c r="C2024" t="inlineStr">
+        <is>
+          <t>Teknik Kimia</t>
+        </is>
+      </c>
+      <c r="D2024" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2024" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2024" t="inlineStr">
+        <is>
+          <t>Baik</t>
+        </is>
+      </c>
+      <c r="G2024" t="n">
+        <v>19</v>
+      </c>
+      <c r="H2024" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2024" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2024" t="n">
+        <v>11</v>
+      </c>
+      <c r="K2024" t="n">
+        <v>330</v>
+      </c>
+      <c r="L2024" t="inlineStr">
+        <is>
+          <t>1:17.37</t>
+        </is>
+      </c>
+    </row>
+    <row r="2025">
+      <c r="A2025" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2025" t="n">
+        <v>352045</v>
+      </c>
+      <c r="C2025" t="inlineStr">
+        <is>
+          <t>Teknik Lingkungan</t>
+        </is>
+      </c>
+      <c r="D2025" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2025" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2025" t="inlineStr">
+        <is>
+          <t>Baik</t>
+        </is>
+      </c>
+      <c r="G2025" t="n">
+        <v>21</v>
+      </c>
+      <c r="H2025" t="n">
+        <v>13</v>
+      </c>
+      <c r="I2025" t="n">
+        <v>2</v>
+      </c>
+      <c r="J2025" t="n">
+        <v>15</v>
+      </c>
+      <c r="K2025" t="n">
+        <v>298</v>
+      </c>
+      <c r="L2025" t="inlineStr">
+        <is>
+          <t>1:14.19</t>
+        </is>
+      </c>
+    </row>
+    <row r="2026">
+      <c r="A2026" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2026" t="n">
+        <v>21201</v>
+      </c>
+      <c r="C2026" t="inlineStr">
+        <is>
+          <t>Teknik Mesin</t>
+        </is>
+      </c>
+      <c r="D2026" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2026" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2026" t="inlineStr">
+        <is>
+          <t>Baik Sekali</t>
+        </is>
+      </c>
+      <c r="G2026" t="n">
+        <v>28</v>
+      </c>
+      <c r="H2026" t="n">
+        <v>16</v>
+      </c>
+      <c r="I2026" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2026" t="n">
+        <v>16</v>
+      </c>
+      <c r="K2026" t="n">
+        <v>698</v>
+      </c>
+      <c r="L2026" t="inlineStr">
+        <is>
+          <t>1:24.93</t>
+        </is>
+      </c>
+    </row>
+    <row r="2027">
+      <c r="A2027" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2027" t="n">
+        <v>21401</v>
+      </c>
+      <c r="C2027" t="inlineStr">
+        <is>
+          <t>Teknik Mesin</t>
+        </is>
+      </c>
+      <c r="D2027" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2027" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+      <c r="F2027" t="inlineStr">
+        <is>
+          <t>Baik</t>
+        </is>
+      </c>
+      <c r="G2027" t="n">
+        <v>15</v>
+      </c>
+      <c r="H2027" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2027" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2027" t="n">
+        <v>7</v>
+      </c>
+      <c r="K2027" t="n">
+        <v>156</v>
+      </c>
+      <c r="L2027" t="inlineStr">
+        <is>
+          <t>1:10.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2028">
+      <c r="A2028" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2028" t="n">
+        <v>22201</v>
+      </c>
+      <c r="C2028" t="inlineStr">
+        <is>
+          <t>Teknik Sipil</t>
+        </is>
+      </c>
+      <c r="D2028" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2028" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2028" t="inlineStr">
+        <is>
+          <t>Baik</t>
+        </is>
+      </c>
+      <c r="G2028" t="n">
+        <v>9</v>
+      </c>
+      <c r="H2028" t="n">
+        <v>11</v>
+      </c>
+      <c r="I2028" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2028" t="n">
+        <v>11</v>
+      </c>
+      <c r="K2028" t="n">
+        <v>115</v>
+      </c>
+      <c r="L2028" t="inlineStr">
+        <is>
+          <t>1:12.78</t>
+        </is>
+      </c>
+    </row>
+    <row r="2029">
+      <c r="A2029" t="inlineStr">
+        <is>
+          <t>Universitas Singaperbangsa Karawang</t>
+        </is>
+      </c>
+      <c r="B2029" t="n">
+        <v>41211</v>
+      </c>
+      <c r="C2029" t="inlineStr">
+        <is>
+          <t>Teknologi Industri Pertanian</t>
+        </is>
+      </c>
+      <c r="D2029" t="inlineStr">
+        <is>
+          <t>Aktif</t>
+        </is>
+      </c>
+      <c r="E2029" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F2029" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2029" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2029" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2029" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2029" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2029" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2029" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>